<commit_message>
Add new Items to MainForm
</commit_message>
<xml_diff>
--- a/TZ.xlsx
+++ b/TZ.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974EB069-D496-4053-AA53-DDF77D2CF083}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3197851-0BA7-4340-8047-3F0B7323D50B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Доработать универсальную форму элемента справочника для списков элементов справочников</t>
   </si>
@@ -41,6 +41,30 @@
   </si>
   <si>
     <t>"=&gt;"</t>
+  </si>
+  <si>
+    <t>Форма "Текущее состояние и местоположение техники"</t>
+  </si>
+  <si>
+    <t>Добавить строку управления таблицами</t>
+  </si>
+  <si>
+    <t>Создать справочник "Место расположения техники"</t>
+  </si>
+  <si>
+    <t>Создать справочник "Ответсвенные лица"</t>
+  </si>
+  <si>
+    <t>Создать документ "Потребность"</t>
+  </si>
+  <si>
+    <t>Создать документ "Закупка"</t>
+  </si>
+  <si>
+    <t>Создать документ "Списание"</t>
+  </si>
+  <si>
+    <t>Создать регистр "Движения техники" Форма "Текущее состояние и местоположение техники"</t>
   </si>
 </sst>
 </file>
@@ -366,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C8"/>
+  <dimension ref="A2:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,6 +445,52 @@
         <v>5</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>45053</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>